<commit_message>
data driven and hardcode separete
</commit_message>
<xml_diff>
--- a/TestCase_Ohrm.xlsx
+++ b/TestCase_Ohrm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Rifat\Project\SQA\OrangeHRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B81BCFD-9ABB-4544-9A14-94B2F2A49260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C3BFB5-B542-417C-828A-1023D2E7A0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="780" windowWidth="13905" windowHeight="12240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenarios" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="68">
   <si>
     <t>Test Scenario (TID)</t>
   </si>
@@ -236,6 +236,21 @@
   </si>
   <si>
     <t>Invalid credentials</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Login successful</t>
+  </si>
+  <si>
+    <t>Invalid credentials eroor</t>
+  </si>
+  <si>
+    <t>Md. Robayet Ahasan Rifat</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -280,7 +295,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +335,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -371,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -406,6 +427,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -879,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C9FA93-7A51-4E04-83B4-24C49FAC5478}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E8" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,10 +1025,18 @@
       <c r="H9" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
+      <c r="I9" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
@@ -1031,10 +1063,18 @@
       <c r="H10" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
+      <c r="I10" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
@@ -1061,10 +1101,18 @@
       <c r="H11" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
+      <c r="I11" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
@@ -1091,10 +1139,18 @@
       <c r="H12" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
+      <c r="I12" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">

</xml_diff>

<commit_message>
new Test Case for T002
</commit_message>
<xml_diff>
--- a/TestCase_Ohrm.xlsx
+++ b/TestCase_Ohrm.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Rifat\Project\SQA\OrangeHRM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Rifat\Project\SQA\OrangeHRM-Selenium-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C3BFB5-B542-417C-828A-1023D2E7A0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D5FAB8-FD8E-4C12-B23C-41CF12C943D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="91">
   <si>
     <t>Test Scenario (TID)</t>
   </si>
@@ -251,6 +251,94 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>1) Launch browser
+2) Open URL "https://opensourcedemo.orangehrmlive.com"
+3) Navigate to Admin &gt; User Management.
+4) Search for a user.
+5) Edit details and save.</t>
+  </si>
+  <si>
+    <t>A new system user should be successfully created, and a success message should appear.</t>
+  </si>
+  <si>
+    <t>The system user details should be updated successfully.</t>
+  </si>
+  <si>
+    <t>The selected user should be deleted, and a success message should appear.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Appropriate error messages should be displayed for the required fields.	</t>
+  </si>
+  <si>
+    <t>The system should display an error message indicating the username already exists.</t>
+  </si>
+  <si>
+    <t>TC_005</t>
+  </si>
+  <si>
+    <t>TC_006</t>
+  </si>
+  <si>
+    <t>TC_007</t>
+  </si>
+  <si>
+    <t>TC_008</t>
+  </si>
+  <si>
+    <t>TC_009</t>
+  </si>
+  <si>
+    <t>Adding a new system user</t>
+  </si>
+  <si>
+    <t>Editing an existing system user</t>
+  </si>
+  <si>
+    <t>Deleting an existing system user</t>
+  </si>
+  <si>
+    <t>Mandatory field validation for adding a new user</t>
+  </si>
+  <si>
+    <t>Duplicate username validation</t>
+  </si>
+  <si>
+    <t>1) Launch browser
+2) Open URL "https://opensourcedemo.orangehrmlive.com"
+3) Log in as Admin
+4) Navigate to Admin &gt; User Management.
+5) Click Add User.
+6) Fill details and save.</t>
+  </si>
+  <si>
+    <t>greatrifat/
+Greatrifat@1</t>
+  </si>
+  <si>
+    <t>Must log in as Admin</t>
+  </si>
+  <si>
+    <t>1) Launch browser
+2) Open URL "https://opensourcedemo.orangehrmlive.com"
+3) Navigate to Admin &gt; User Management.
+4) Search for the user.
+5) Select the user and click Delete</t>
+  </si>
+  <si>
+    <t>greatrifat</t>
+  </si>
+  <si>
+    <t>1) Launch browser
+2) Open URL "https://opensourcedemo.orangehrmlive.com"
+3) Navigate to Admin &gt; User Management.
+1. Click Add User.
+2. Leave mandatory fields blank.
+3. Click Save</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Must have a user with same username </t>
   </si>
 </sst>
 </file>
@@ -295,7 +383,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,6 +429,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -392,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -423,14 +517,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -721,7 +827,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,17 +1007,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C9FA93-7A51-4E04-83B4-24C49FAC5478}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="18.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="5" customWidth="1"/>
     <col min="4" max="4" width="52.7109375" style="5" customWidth="1"/>
     <col min="5" max="5" width="27.28515625" style="5" customWidth="1"/>
     <col min="6" max="6" width="47.140625" style="5" customWidth="1"/>
@@ -925,10 +1031,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="13"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D2" s="3" t="s">
@@ -1028,7 +1134,7 @@
       <c r="I9" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="12" t="s">
         <v>63</v>
       </c>
       <c r="K9" s="11" t="s">
@@ -1066,7 +1172,7 @@
       <c r="I10" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="12" t="s">
         <v>63</v>
       </c>
       <c r="K10" s="11" t="s">
@@ -1104,7 +1210,7 @@
       <c r="I11" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="12" t="s">
         <v>63</v>
       </c>
       <c r="K11" s="11" t="s">
@@ -1142,7 +1248,7 @@
       <c r="I12" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="12" t="s">
         <v>63</v>
       </c>
       <c r="K12" s="11" t="s">
@@ -1152,91 +1258,151 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
+        <v>74</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>69</v>
+      </c>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+        <v>75</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>70</v>
+      </c>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
+        <v>76</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
+        <v>77</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>73</v>
+      </c>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
+        <v>78</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
@@ -1494,24 +1660,6 @@
       <c r="K31" s="11"/>
       <c r="L31" s="11"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:E1"/>

</xml_diff>